<commit_message>
contourmaps interpolated values area1
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/interpolation/Feature_engineering/combined/Area1_counts.xlsx
+++ b/_CLUSTER/groups_time_area/interpolation/Feature_engineering/combined/Area1_counts.xlsx
@@ -375,7 +375,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>36400</v>
@@ -383,7 +383,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B3" t="n">
         <v>14117</v>
@@ -391,7 +391,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>3913</v>
@@ -399,7 +399,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
         <v>983</v>

</xml_diff>